<commit_message>
Upload de versão funcional da API
</commit_message>
<xml_diff>
--- a/Backlog - Projeto Individual.xlsx
+++ b/Backlog - Projeto Individual.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7420E306-1639-4E45-8472-74791150D91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\Documents\SP Tech\CCO\Projeto\Projeto-EU_AOS_PEDACOS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EAFF1D-5C5E-4DF4-9770-F57AD87F8ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$1:$M$17</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>REQUISITOS</t>
   </si>
@@ -181,12 +186,6 @@
   </si>
   <si>
     <t>Importante</t>
-  </si>
-  <si>
-    <t>Hospedagem de Site na VM</t>
-  </si>
-  <si>
-    <t>Hospedagem dos arquivos do site em Máquina Virtual, utilizando a Oracle VirtualBox.</t>
   </si>
   <si>
     <t>Hospedagem de Banco de Dados na VM</t>
@@ -205,7 +204,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +224,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -290,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
@@ -316,6 +323,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +475,10 @@
                   <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>199</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -535,16 +543,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1306,7 +1314,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1669,28 +1677,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="B1:M18"/>
+  <dimension ref="B1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="49.85546875" customWidth="1"/>
-    <col min="3" max="3" width="81.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.88671875" customWidth="1"/>
+    <col min="3" max="3" width="81.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.75">
+    <row r="1" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1725,7 +1732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:13">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1759,10 +1766,10 @@
       </c>
       <c r="M2" s="3">
         <f>SUMIFS($F:$F, $H:$H, K2, $I:$I, "VERDADEIRO")</f>
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="2:13">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1785,7 +1792,7 @@
         <v>14</v>
       </c>
       <c r="I3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>18</v>
@@ -1796,10 +1803,10 @@
       </c>
       <c r="M3" s="1">
         <f>SUMIFS($F:$F, $H:$H, K3, $I:$I, "VERDADEIRO")</f>
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1822,21 +1829,21 @@
         <v>14</v>
       </c>
       <c r="I4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="L4" s="1">
         <f>SUMIF($H:$H,K4,$F:$F)</f>
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="M4" s="1">
         <f>SUMIFS($F:$F, $H:$H, K4, $I:$I, "VERDADEIRO")</f>
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1866,14 +1873,14 @@
       </c>
       <c r="L5" s="1">
         <f>SUM(L2:L4)</f>
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="M5" s="1">
         <f>SUM(M2:M4)</f>
-        <v>9</v>
+        <v>142</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1899,7 +1906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:13" hidden="1">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1922,10 +1929,10 @@
         <v>22</v>
       </c>
       <c r="I7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:13" hidden="1">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1948,10 +1955,10 @@
         <v>22</v>
       </c>
       <c r="I8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:13" hidden="1">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1977,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
@@ -2000,10 +2007,10 @@
         <v>14</v>
       </c>
       <c r="I10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
@@ -2026,10 +2033,10 @@
         <v>14</v>
       </c>
       <c r="I11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:13" hidden="1">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
@@ -2055,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:13" hidden="1">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>41</v>
       </c>
@@ -2078,10 +2085,10 @@
         <v>18</v>
       </c>
       <c r="I13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:13" hidden="1">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
@@ -2104,10 +2111,10 @@
         <v>22</v>
       </c>
       <c r="I14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:13" hidden="1">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
@@ -2133,7 +2140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:13" hidden="1">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
@@ -2159,7 +2166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:9" hidden="1">
+    <row r="17" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>51</v>
       </c>
@@ -2170,56 +2177,28 @@
         <v>12</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F17" s="1">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G17" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="18.75" hidden="1" customHeight="1">
-      <c r="B18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="1">
-        <v>21</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I24" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:M18" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Sprint 1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:M17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>